<commit_message>
Updated Graph to include a log version also
</commit_message>
<xml_diff>
--- a/Project_1/Graph of nodes expanded.xlsx
+++ b/Project_1/Graph of nodes expanded.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26300" windowHeight="15000"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="26240" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,8 +112,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,7 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -165,6 +167,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -180,6 +183,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -227,7 +231,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.203742426264514"/>
+          <c:y val="0.00557103064066852"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -237,8 +248,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0830100041842596"/>
-          <c:y val="0.0981912144702842"/>
+          <c:x val="0.0911111704257307"/>
+          <c:y val="0.0929397056565701"/>
           <c:w val="0.815021872265967"/>
           <c:h val="0.763087082650138"/>
         </c:manualLayout>
@@ -251,7 +262,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -265,7 +276,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -288,7 +299,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$H$2</c:f>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -317,7 +328,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
+              <c:f>Sheet1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -331,7 +342,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -354,7 +365,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$H$3</c:f>
+              <c:f>Sheet1!$C$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -383,7 +394,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -397,7 +408,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -420,7 +431,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$H$4</c:f>
+              <c:f>Sheet1!$C$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -449,7 +460,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$5</c:f>
+              <c:f>Sheet1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -463,7 +474,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -486,7 +497,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$H$5</c:f>
+              <c:f>Sheet1!$C$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -515,7 +526,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>Sheet1!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -529,7 +540,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -552,7 +563,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$H$6</c:f>
+              <c:f>Sheet1!$C$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -581,7 +592,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$7</c:f>
+              <c:f>Sheet1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -595,7 +606,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$1:$H$1</c:f>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -618,7 +629,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$H$7</c:f>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -652,11 +663,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094586952"/>
-        <c:axId val="2094349464"/>
+        <c:axId val="2076361496"/>
+        <c:axId val="2076368456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2094586952"/>
+        <c:axId val="2076361496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094349464"/>
+        <c:crossAx val="2076368456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -693,7 +704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094349464"/>
+        <c:axId val="2076368456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094586952"/>
+        <c:crossAx val="2076361496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -745,19 +756,604 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graph</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Nodes expanded (log axis) vs World explored</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.124253531936667"/>
+          <c:y val="0.0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.104737769692146"/>
+          <c:y val="0.0764501663227925"/>
+          <c:w val="0.815021872265967"/>
+          <c:h val="0.763087082650138"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>259.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>357.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1159.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>890.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>129.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>189.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>553.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>587.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>world 1 -- trivial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>world 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>world 3 -- moderate size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>world 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>world 5 -- very large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>190.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2088334760"/>
+        <c:axId val="2089899640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2088334760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>World Types</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2089899640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2089899640"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Number of Nodes expanded</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>(log axis)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0"/>
+              <c:y val="0.237603899111542"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2088334760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.923606128656301"/>
+          <c:y val="0.38248999957893"/>
+          <c:w val="0.0757105630132548"/>
+          <c:h val="0.320472022114257"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -772,6 +1368,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1067,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1086,143 +1714,143 @@
     <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:7">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1">
+        <v>259</v>
+      </c>
       <c r="D2" s="1">
-        <v>259</v>
+        <v>168</v>
       </c>
       <c r="E2" s="1">
-        <v>168</v>
+        <v>357</v>
       </c>
       <c r="F2" s="1">
-        <v>357</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1">
-        <v>74</v>
-      </c>
-      <c r="H2" s="1">
         <v>1159</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:7">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1">
+        <v>188</v>
+      </c>
       <c r="D3" s="1">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="E3" s="1">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="F3" s="1">
-        <v>250</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1">
-        <v>56</v>
-      </c>
-      <c r="H3" s="1">
         <v>890</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:7">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1">
+        <v>129</v>
+      </c>
       <c r="D4" s="1">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1">
-        <v>85</v>
+        <v>271</v>
       </c>
       <c r="F4" s="1">
-        <v>271</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1">
-        <v>58</v>
-      </c>
-      <c r="H4" s="1">
         <v>720</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:7">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="1">
+        <v>95</v>
+      </c>
       <c r="D5" s="1">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1">
+        <v>189</v>
+      </c>
+      <c r="F5" s="1">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
         <v>95</v>
       </c>
-      <c r="E5" s="1">
-        <v>67</v>
-      </c>
-      <c r="F5" s="1">
-        <v>189</v>
-      </c>
-      <c r="G5" s="1">
-        <v>39</v>
-      </c>
-      <c r="H5" s="1">
-        <v>553</v>
+      <c r="D6" s="1">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1">
+        <v>191</v>
+      </c>
+      <c r="F6" s="1">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1">
+        <v>587</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1">
-        <v>95</v>
-      </c>
-      <c r="E6" s="1">
-        <v>62</v>
-      </c>
-      <c r="F6" s="1">
-        <v>191</v>
-      </c>
-      <c r="G6" s="1">
-        <v>36</v>
-      </c>
-      <c r="H6" s="1">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="1:7">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
       <c r="D7" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reordering worlds in writeup and Graph of nodes expanded
</commit_message>
<xml_diff>
--- a/Project_1/Graph of nodes expanded.xlsx
+++ b/Project_1/Graph of nodes expanded.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="26240" windowHeight="15000"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="24280" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,8 +112,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -151,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +180,12 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -184,6 +202,12 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -271,9 +295,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -304,16 +325,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>259.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>357.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>168.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>357.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>74.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1159.0</c:v>
@@ -337,9 +358,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -370,16 +388,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>188.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>890.0</c:v>
@@ -403,9 +421,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -436,16 +451,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>129.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>271.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>720.0</c:v>
@@ -469,9 +484,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -502,16 +514,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>189.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>189.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>553.0</c:v>
@@ -535,9 +547,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -568,16 +577,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>191.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>587.0</c:v>
@@ -601,9 +610,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -634,16 +640,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>190.0</c:v>
@@ -663,11 +669,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2076361496"/>
-        <c:axId val="2076368456"/>
+        <c:axId val="2083491064"/>
+        <c:axId val="2088489816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2076361496"/>
+        <c:axId val="2083491064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076368456"/>
+        <c:crossAx val="2088489816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -704,7 +710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076368456"/>
+        <c:axId val="2088489816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076361496"/>
+        <c:crossAx val="2083491064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -831,9 +837,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -864,16 +867,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>259.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>357.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>168.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>357.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>74.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1159.0</c:v>
@@ -897,9 +900,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -930,16 +930,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>188.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>890.0</c:v>
@@ -963,9 +963,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -996,16 +993,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>129.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>271.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>720.0</c:v>
@@ -1029,9 +1026,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -1062,16 +1056,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>189.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>189.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>553.0</c:v>
@@ -1095,9 +1089,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -1128,16 +1119,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>191.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>191.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>587.0</c:v>
@@ -1161,9 +1152,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
@@ -1194,16 +1182,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>190.0</c:v>
@@ -1223,11 +1211,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088334760"/>
-        <c:axId val="2089899640"/>
+        <c:axId val="2043442328"/>
+        <c:axId val="2030014776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088334760"/>
+        <c:axId val="2043442328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,7 +1244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089899640"/>
+        <c:crossAx val="2030014776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1264,7 +1252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089899640"/>
+        <c:axId val="2030014776"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1310,7 +1298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088334760"/>
+        <c:crossAx val="2043442328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1698,7 +1686,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1739,16 +1727,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1">
         <v>259</v>
-      </c>
-      <c r="D2" s="1">
-        <v>168</v>
       </c>
       <c r="E2" s="1">
         <v>357</v>
       </c>
       <c r="F2" s="1">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="G2" s="1">
         <v>1159</v>
@@ -1759,16 +1747,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1">
         <v>188</v>
-      </c>
-      <c r="D3" s="1">
-        <v>128</v>
       </c>
       <c r="E3" s="1">
         <v>250</v>
       </c>
       <c r="F3" s="1">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="G3" s="1">
         <v>890</v>
@@ -1779,16 +1767,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1">
         <v>129</v>
-      </c>
-      <c r="D4" s="1">
-        <v>85</v>
       </c>
       <c r="E4" s="1">
         <v>271</v>
       </c>
       <c r="F4" s="1">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="G4" s="1">
         <v>720</v>
@@ -1799,16 +1787,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1">
         <v>95</v>
-      </c>
-      <c r="D5" s="1">
-        <v>67</v>
       </c>
       <c r="E5" s="1">
         <v>189</v>
       </c>
       <c r="F5" s="1">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G5" s="1">
         <v>553</v>
@@ -1819,16 +1807,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1">
         <v>95</v>
-      </c>
-      <c r="D6" s="1">
-        <v>62</v>
       </c>
       <c r="E6" s="1">
         <v>191</v>
       </c>
       <c r="F6" s="1">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1">
         <v>587</v>
@@ -1839,16 +1827,16 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
         <v>12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>11</v>
       </c>
       <c r="E7" s="1">
         <v>66</v>
       </c>
       <c r="F7" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>190</v>

</xml_diff>